<commit_message>
add document comment in xlsx file
</commit_message>
<xml_diff>
--- a/rawresource/rawconfig/dungeon.xlsx
+++ b/rawresource/rawconfig/dungeon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8640" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8640" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <author>xzc</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0">
+    <comment ref="G3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
+  <si>
+    <t>副本配置</t>
+  </si>
   <si>
     <t>array</t>
   </si>
@@ -148,6 +151,9 @@
     <t>{10}</t>
   </si>
   <si>
+    <t>场景配置</t>
+  </si>
+  <si>
     <t>场景id</t>
   </si>
   <si>
@@ -248,6 +254,9 @@
   </si>
   <si>
     <t>max_y</t>
+  </si>
+  <si>
+    <t>区域属性配置</t>
   </si>
   <si>
     <t>区域属性id</t>
@@ -282,10 +291,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -293,13 +302,6 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -311,6 +313,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,25 +346,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -368,7 +362,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,14 +401,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -407,14 +408,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,6 +422,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -435,11 +437,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -460,31 +469,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,151 +643,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,6 +691,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -692,21 +716,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -723,16 +732,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,138 +768,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1214,7 +1223,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
@@ -1247,175 +1256,180 @@
     <col min="26" max="1025" width="8.69166666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17">
         <v>10</v>
       </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C17" t="s">
         <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1428,10 +1442,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1442,159 +1456,118 @@
     <col min="6" max="6" width="13.3916666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H6" t="s">
         <v>47</v>
-      </c>
-      <c r="E5">
-        <v>64</v>
-      </c>
-      <c r="F5">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6">
-        <v>64</v>
-      </c>
-      <c r="F6">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
       </c>
       <c r="E7">
         <v>64</v>
@@ -1603,21 +1576,21 @@
         <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>64</v>
@@ -1626,21 +1599,21 @@
         <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>64</v>
@@ -1649,21 +1622,21 @@
         <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <v>64</v>
@@ -1672,21 +1645,21 @@
         <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E11">
         <v>64</v>
@@ -1695,21 +1668,21 @@
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E12">
         <v>64</v>
@@ -1718,21 +1691,21 @@
         <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13">
         <v>64</v>
@@ -1741,21 +1714,21 @@
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E14">
         <v>64</v>
@@ -1764,9 +1737,55 @@
         <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <v>64</v>
+      </c>
+      <c r="F15">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16">
         <v>10</v>
       </c>
     </row>
@@ -1779,10 +1798,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -1792,120 +1811,85 @@
     <col min="7" max="7" width="12.825" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>65</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D5" t="s">
         <v>66</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>64</v>
-      </c>
-      <c r="G5">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>64</v>
-      </c>
-      <c r="G6">
-        <v>128</v>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -1925,7 +1909,7 @@
     </row>
     <row r="8" spans="2:7">
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -1945,7 +1929,7 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -1965,7 +1949,7 @@
     </row>
     <row r="10" spans="2:7">
       <c r="B10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -1985,7 +1969,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>50</v>
@@ -2005,7 +1989,7 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -2025,7 +2009,7 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>50</v>
@@ -2045,7 +2029,7 @@
     </row>
     <row r="14" spans="2:7">
       <c r="B14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>50</v>
@@ -2060,6 +2044,46 @@
         <v>64</v>
       </c>
       <c r="G14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>64</v>
+      </c>
+      <c r="G15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>64</v>
+      </c>
+      <c r="G16">
         <v>128</v>
       </c>
     </row>
@@ -2072,10 +2096,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -2083,154 +2107,159 @@
     <col min="7" max="7" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
         <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>66</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D5" t="s">
         <v>67</v>
       </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>66</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D6" t="s">
         <v>67</v>
       </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6">
-        <v>2</v>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16">
         <v>10</v>
       </c>
     </row>

</xml_diff>